<commit_message>
Evaluation results and configuration tested updated
</commit_message>
<xml_diff>
--- a/Evaluation_Results.xlsx
+++ b/Evaluation_Results.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrea\Desktop\UBC Research Period\Research\0_Latest Version\Data Chart Captioning System\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43E22173-2324-4F38-90DB-9DD0EF9A93D6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48084B07-BEBC-47B6-9214-17A7ECDBD63E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" xr2:uid="{1019824F-6233-490B-85E9-0CFFF39F141C}"/>
+    <workbookView xWindow="47880" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{1019824F-6233-490B-85E9-0CFFF39F141C}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
+    <sheet name="Foglio2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="77">
   <si>
     <t>Sentence Generation</t>
   </si>
@@ -214,13 +215,61 @@
   </si>
   <si>
     <t>15.47</t>
+  </si>
+  <si>
+    <t>Configuration #</t>
+  </si>
+  <si>
+    <t>Dropout</t>
+  </si>
+  <si>
+    <t>Optimizer</t>
+  </si>
+  <si>
+    <t>Lr</t>
+  </si>
+  <si>
+    <t>Epochs</t>
+  </si>
+  <si>
+    <t>Batch Size</t>
+  </si>
+  <si>
+    <t>LSTM Units</t>
+  </si>
+  <si>
+    <t>Embed size</t>
+  </si>
+  <si>
+    <t>0.2</t>
+  </si>
+  <si>
+    <t>39.17</t>
+  </si>
+  <si>
+    <t>41.88</t>
+  </si>
+  <si>
+    <t>35.90</t>
+  </si>
+  <si>
+    <t>80.77</t>
+  </si>
+  <si>
+    <t>S-F1-AVG-L</t>
+  </si>
+  <si>
+    <t>S-F1-Best-L</t>
+  </si>
+  <si>
+    <t>Adam</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -236,13 +285,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -298,7 +367,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -306,6 +375,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -315,19 +408,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -646,8 +760,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6F245F8-9BDD-47E4-A555-645AEBF9C027}">
   <dimension ref="A3:O11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10:J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -661,63 +775,63 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="4" t="s">
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="4" t="s">
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
+      <c r="M3" s="12"/>
+      <c r="N3" s="12"/>
+      <c r="O3" s="12"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="7" t="s">
+      <c r="C4" s="13"/>
+      <c r="D4" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="3"/>
+      <c r="E4" s="11"/>
       <c r="F4" s="1"/>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3" t="s">
+      <c r="H4" s="11"/>
+      <c r="I4" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="J4" s="3"/>
+      <c r="J4" s="11"/>
       <c r="K4" s="1"/>
-      <c r="L4" s="3" t="s">
+      <c r="L4" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3" t="s">
+      <c r="M4" s="11"/>
+      <c r="N4" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="O4" s="3"/>
+      <c r="O4" s="11"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="4" t="s">
         <v>2</v>
       </c>
       <c r="E5" s="2" t="s">
@@ -757,23 +871,23 @@
       <c r="B6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="10" t="s">
         <v>31</v>
       </c>
       <c r="F6" s="1"/>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="H6" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="I6" s="8" t="s">
+      <c r="I6" s="4" t="s">
         <v>49</v>
       </c>
       <c r="J6" s="2" t="s">
@@ -781,8 +895,8 @@
       </c>
       <c r="K6" s="1"/>
       <c r="L6" s="2"/>
-      <c r="M6" s="6"/>
-      <c r="N6" s="8"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="4"/>
       <c r="O6" s="2"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.55000000000000004">
@@ -792,7 +906,7 @@
       <c r="B7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D7" s="8" t="s">
@@ -802,22 +916,22 @@
         <v>32</v>
       </c>
       <c r="F7" s="1"/>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H7" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="I7" s="8" t="s">
+      <c r="I7" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="J7" s="10" t="s">
         <v>56</v>
       </c>
       <c r="K7" s="1"/>
       <c r="L7" s="2"/>
-      <c r="M7" s="6"/>
-      <c r="N7" s="8"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="4"/>
       <c r="O7" s="2"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.55000000000000004">
@@ -827,32 +941,32 @@
       <c r="B8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="9" t="s">
         <v>27</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>33</v>
       </c>
       <c r="F8" s="1"/>
-      <c r="G8" s="2" t="s">
+      <c r="G8" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="H8" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="I8" s="8" t="s">
+      <c r="I8" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="J8" s="10" t="s">
         <v>57</v>
       </c>
       <c r="K8" s="1"/>
       <c r="L8" s="2"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="8"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="4"/>
       <c r="O8" s="2"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.55000000000000004">
@@ -862,7 +976,7 @@
       <c r="B9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="3" t="s">
         <v>22</v>
       </c>
       <c r="D9" s="8" t="s">
@@ -872,57 +986,57 @@
         <v>34</v>
       </c>
       <c r="F9" s="1"/>
-      <c r="G9" s="2" t="s">
+      <c r="G9" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="H9" s="6" t="s">
+      <c r="H9" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="I9" s="8" t="s">
+      <c r="I9" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="J9" s="10" t="s">
         <v>58</v>
       </c>
       <c r="K9" s="1"/>
       <c r="L9" s="2"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="8"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="4"/>
       <c r="O9" s="2"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="F10" s="1"/>
-      <c r="G10" s="2" t="s">
+      <c r="F10" s="5"/>
+      <c r="G10" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="H10" s="6" t="s">
+      <c r="H10" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="I10" s="8" t="s">
+      <c r="I10" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="J10" s="2" t="s">
+      <c r="J10" s="6" t="s">
         <v>59</v>
       </c>
       <c r="K10" s="1"/>
       <c r="L10" s="2"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="8"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="4"/>
       <c r="O10" s="2"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.55000000000000004">
@@ -932,23 +1046,23 @@
       <c r="B11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="3" t="s">
         <v>24</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="10" t="s">
         <v>36</v>
       </c>
       <c r="F11" s="1"/>
-      <c r="G11" s="2" t="s">
+      <c r="G11" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="H11" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="I11" s="8" t="s">
+      <c r="I11" s="4" t="s">
         <v>54</v>
       </c>
       <c r="J11" s="2" t="s">
@@ -956,8 +1070,8 @@
       </c>
       <c r="K11" s="1"/>
       <c r="L11" s="2"/>
-      <c r="M11" s="6"/>
-      <c r="N11" s="8"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="4"/>
       <c r="O11" s="2"/>
     </row>
   </sheetData>
@@ -975,4 +1089,331 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6A2D0E8-00E4-4E70-AB49-CDE972218ED4}">
+  <dimension ref="B4:N18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="2" max="2" width="16.26171875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.734375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.1015625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.9453125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.9453125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.3125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.26171875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5234375" customWidth="1"/>
+    <col min="10" max="10" width="6.9453125" customWidth="1"/>
+    <col min="11" max="14" width="12.578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:14" s="16" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B4" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="I4" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="J4" s="19"/>
+      <c r="K4" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="L4" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="M4" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="N4" s="15" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" s="16" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B5" s="17">
+        <v>5</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="E5" s="18">
+        <v>1E-3</v>
+      </c>
+      <c r="F5" s="18">
+        <v>300</v>
+      </c>
+      <c r="G5" s="18">
+        <v>64</v>
+      </c>
+      <c r="H5" s="18">
+        <v>128</v>
+      </c>
+      <c r="I5" s="18">
+        <v>128</v>
+      </c>
+      <c r="J5" s="20"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="18"/>
+      <c r="M5" s="18"/>
+      <c r="N5" s="18"/>
+    </row>
+    <row r="6" spans="2:14" s="16" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B6" s="17">
+        <v>6</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="E6" s="18">
+        <v>1E-4</v>
+      </c>
+      <c r="F6" s="18">
+        <v>300</v>
+      </c>
+      <c r="G6" s="18">
+        <v>64</v>
+      </c>
+      <c r="H6" s="18">
+        <v>128</v>
+      </c>
+      <c r="I6" s="18">
+        <v>128</v>
+      </c>
+      <c r="J6" s="20"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="18"/>
+      <c r="N6" s="18"/>
+    </row>
+    <row r="7" spans="2:14" s="16" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B7" s="17">
+        <v>8</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="E7" s="18">
+        <v>1E-3</v>
+      </c>
+      <c r="F7" s="18">
+        <v>150</v>
+      </c>
+      <c r="G7" s="18">
+        <v>64</v>
+      </c>
+      <c r="H7" s="18">
+        <v>64</v>
+      </c>
+      <c r="I7" s="18">
+        <v>128</v>
+      </c>
+      <c r="J7" s="20"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="18"/>
+      <c r="M7" s="18"/>
+      <c r="N7" s="18"/>
+    </row>
+    <row r="8" spans="2:14" s="16" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B8" s="17">
+        <v>10</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="E8" s="18">
+        <v>1E-3</v>
+      </c>
+      <c r="F8" s="18">
+        <v>150</v>
+      </c>
+      <c r="G8" s="18">
+        <v>32</v>
+      </c>
+      <c r="H8" s="18">
+        <v>64</v>
+      </c>
+      <c r="I8" s="18">
+        <v>128</v>
+      </c>
+      <c r="J8" s="20"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="18"/>
+      <c r="M8" s="18"/>
+      <c r="N8" s="18"/>
+    </row>
+    <row r="9" spans="2:14" s="16" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B9" s="17">
+        <v>11</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="E9" s="18">
+        <v>1E-3</v>
+      </c>
+      <c r="F9" s="18">
+        <v>150</v>
+      </c>
+      <c r="G9" s="18">
+        <v>16</v>
+      </c>
+      <c r="H9" s="18">
+        <v>64</v>
+      </c>
+      <c r="I9" s="18">
+        <v>128</v>
+      </c>
+      <c r="J9" s="20"/>
+      <c r="K9" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="L9" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="M9" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="N9" s="18" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" ht="21" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B10" s="17">
+        <v>12</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="E10" s="18">
+        <v>1E-3</v>
+      </c>
+      <c r="F10" s="18">
+        <v>150</v>
+      </c>
+      <c r="G10" s="18">
+        <v>8</v>
+      </c>
+      <c r="H10" s="18">
+        <v>64</v>
+      </c>
+      <c r="I10" s="18">
+        <v>128</v>
+      </c>
+      <c r="J10" s="20"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="18"/>
+      <c r="N10" s="18"/>
+    </row>
+    <row r="11" spans="2:14" ht="21" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B11" s="17">
+        <v>13</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="E11" s="18">
+        <v>1E-3</v>
+      </c>
+      <c r="F11" s="18">
+        <v>150</v>
+      </c>
+      <c r="G11" s="18">
+        <v>16</v>
+      </c>
+      <c r="H11" s="18">
+        <v>128</v>
+      </c>
+      <c r="I11" s="18">
+        <v>128</v>
+      </c>
+      <c r="J11" s="20"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="18"/>
+      <c r="M11" s="18"/>
+      <c r="N11" s="18"/>
+    </row>
+    <row r="12" spans="2:14" ht="21" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B12" s="17"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="18"/>
+      <c r="L12" s="18"/>
+      <c r="M12" s="18"/>
+      <c r="N12" s="18"/>
+    </row>
+    <row r="13" spans="2:14" ht="21" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B13" s="17"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="18"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="18"/>
+      <c r="L13" s="18"/>
+      <c r="M13" s="18"/>
+      <c r="N13" s="18"/>
+    </row>
+    <row r="14" spans="2:14" ht="21" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="15" spans="2:14" ht="21" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="16" spans="2:14" ht="21" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="17" ht="21" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="18" ht="21" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>